<commit_message>
Completed Registeration, Change login page, added forget password and change password facility
</commit_message>
<xml_diff>
--- a/AluminiConnect/scripts/acc.xlsx
+++ b/AluminiConnect/scripts/acc.xlsx
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t xml:space="preserve">roll_no</t>
   </si>
   <si>
-    <t xml:space="preserve">first_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last_name</t>
+    <t xml:space="preserve">name</t>
   </si>
   <si>
     <t xml:space="preserve">email</t>
@@ -49,58 +46,46 @@
     <t xml:space="preserve">batch</t>
   </si>
   <si>
-    <t xml:space="preserve">Arpan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tarkas</t>
+    <t xml:space="preserve">Arpan Tarkas</t>
   </si>
   <si>
     <t xml:space="preserve">2016049@iiitdmj.ac.in</t>
   </si>
   <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namit Pai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016178@iiitdmj.ac.in</t>
+  </si>
+  <si>
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">B.Tech</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016178@iiitdmj.ac.in</t>
-  </si>
-  <si>
     <t xml:space="preserve">CSE</t>
   </si>
   <si>
-    <t xml:space="preserve">Tushar</t>
+    <t xml:space="preserve">Tushar Srivastava</t>
   </si>
   <si>
     <t xml:space="preserve">2016280@iiitdmj.ac.in</t>
   </si>
   <si>
-    <t xml:space="preserve">Mudit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joshi</t>
+    <t xml:space="preserve">Mudit Joshi</t>
   </si>
   <si>
     <t xml:space="preserve">2016162@iiitdmj.ac.in</t>
   </si>
   <si>
     <t xml:space="preserve">ECE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fuddi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016100@iiitdmj.ac.in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
   </si>
 </sst>
 </file>
@@ -213,19 +198,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -253,162 +239,117 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>2016049</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="n">
+        <v>36021</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>36021</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>2020</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2016178</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="2" t="n">
+        <v>36022</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>36022</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>2019</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>2016280</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="n">
+      <c r="E4" s="2" t="n">
         <v>36023</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>2020</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>2016162</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>36024</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>36024</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>2016100</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>36025</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>2020</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="2016049@iiitdmj.ac.in"/>
-    <hyperlink ref="D3" r:id="rId2" display="2016178@iiitdmj.ac.in"/>
-    <hyperlink ref="D4" r:id="rId3" display="2016280@iiitdmj.ac.in"/>
-    <hyperlink ref="D5" r:id="rId4" display="2016162@iiitdmj.ac.in"/>
-    <hyperlink ref="D6" r:id="rId5" display="2016100@iiitdmj.ac.in"/>
+    <hyperlink ref="C2" r:id="rId1" display="2016049@iiitdmj.ac.in"/>
+    <hyperlink ref="C3" r:id="rId2" display="2016178@iiitdmj.ac.in"/>
+    <hyperlink ref="C4" r:id="rId3" display="2016280@iiitdmj.ac.in"/>
+    <hyperlink ref="C5" r:id="rId4" display="2016162@iiitdmj.ac.in"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>